<commit_message>
nouveau diagramme de gantt
</commit_message>
<xml_diff>
--- a/projet-/01-Preproduction/Diagramme de gantt de Mbieleu Honore apllication mobile.xlsx
+++ b/projet-/01-Preproduction/Diagramme de gantt de Mbieleu Honore apllication mobile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Etapes</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Hebergement sur playstore</t>
+  </si>
+  <si>
+    <t>Maintenace</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -167,9 +177,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$8</c:f>
+              <c:f>Feuil1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Etude de marche(analyse)</c:v>
                 </c:pt>
@@ -190,36 +200,42 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Hebergement sur playstore</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenace</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$8</c:f>
+              <c:f>Feuil1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>45099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45102</c:v>
+                  <c:v>45105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45105</c:v>
+                  <c:v>45109</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45120</c:v>
+                  <c:v>45128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45128</c:v>
+                  <c:v>45143</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45131</c:v>
+                  <c:v>45149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45133</c:v>
+                  <c:v>45151</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -243,30 +259,33 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$2:$C$8</c:f>
+              <c:f>Feuil1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,7 +359,7 @@
         <c:axId val="1028016384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45134"/>
+          <c:max val="45165"/>
           <c:min val="45099"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1019,6 +1038,23 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Etapes"/>
+    <tableColumn id="2" name="Date de debut" dataDxfId="1">
+      <calculatedColumnFormula>+D1+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Duree (en jour)"/>
+    <tableColumn id="4" name="Date de fin" dataDxfId="0">
+      <calculatedColumnFormula>+C2+B2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -1282,17 +1318,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,11 +1354,11 @@
         <v>45099</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <f>+C2+B2</f>
-        <v>45101</v>
+        <v>45104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1330,14 +1367,14 @@
       </c>
       <c r="B3" s="2">
         <f>+D2+1</f>
-        <v>45102</v>
+        <v>45105</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D8" si="0">+C3+B3</f>
-        <v>45104</v>
+        <f t="shared" ref="D3:D9" si="0">+C3+B3</f>
+        <v>45108</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,14 +1383,14 @@
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:B8" si="1">+D3+1</f>
-        <v>45105</v>
+        <v>45109</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>45119</v>
+        <v>45127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1362,14 +1399,14 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" si="1"/>
-        <v>45120</v>
+        <v>45128</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>45127</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,14 +1415,14 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" si="1"/>
-        <v>45128</v>
+        <v>45143</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>45130</v>
+        <v>45148</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1394,14 +1431,14 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" si="1"/>
-        <v>45131</v>
+        <v>45149</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>45132</v>
+        <v>45150</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,18 +1447,37 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" si="1"/>
-        <v>45133</v>
+        <v>45151</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>45134</v>
+        <v>45152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <f>+D8+1</f>
+        <v>45153</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2">
+        <f>+C9+B9</f>
+        <v>45183</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>